<commit_message>
references & sheet updates
</commit_message>
<xml_diff>
--- a/delta2/lib_e/dfir_osir/dfir_20220808.xlsx
+++ b/delta2/lib_e/dfir_osir/dfir_20220808.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harveywargo/Desktop/GithubProjects/h2w-delta/delta2/lib_e/dfir_osir/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23942935-4E0C-4549-8E6A-038236704EDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58851098-686E-0F48-912E-2F1D629745C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{2B361B8B-B20C-1B4A-9CA2-9DEA1E5C6017}"/>
+    <workbookView xWindow="0" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{2B361B8B-B20C-1B4A-9CA2-9DEA1E5C6017}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="239">
   <si>
     <t>eid</t>
   </si>
@@ -591,9 +591,6 @@
     <t>dfir20220808-eid0089</t>
   </si>
   <si>
-    <t>{"sigma_uuid": "4358e5a5-7542-4dcb-b9f3-87667371839b", "sigma_title": "ISO or Image Mount Indicator in Recent Files"}</t>
-  </si>
-  <si>
     <t>{"sigma_uuid": "0248a7bc-8a9a-4cd8-a57e-3ae8e073a073", "sigma_title": "ISO Image Mount"}</t>
   </si>
   <si>
@@ -687,21 +684,6 @@
     <t>dfir20220808-eid0105</t>
   </si>
   <si>
-    <t>ET POLICY OpenSSL Demo CA - Internet Widgits Pty (O)
-ET POLICY SMB Executable File Transfer
-ET RPC DCERPC SVCCTL - Remote Service Control Manager Access
-ET POLICY SMB2 NT Create AndX Request For an Executable File
-ET POLICY SSL/TLS Certificate Observed (AnyDesk Remote Desktop Software)
-ET USER_AGENTS AnyDesk Remote Desktop Software User-Agent
-(Snort VRT) MALWARE-OTHER CobaltStrike powershell web delivery attempt</t>
-  </si>
-  <si>
-    <t>generic</t>
-  </si>
-  <si>
-    <t>et_rule</t>
-  </si>
-  <si>
     <t>eid_type</t>
   </si>
   <si>
@@ -711,9 +693,6 @@
     <t>ET USER_AGENTS AnyDesk Remote Desktop Software User-Agent</t>
   </si>
   <si>
-    <t>ET POLICY SSL/TLS Certificate Observed (AnyDesk Remote Desktop Software</t>
-  </si>
-  <si>
     <t>object_sigma</t>
   </si>
   <si>
@@ -724,6 +703,57 @@
   </si>
   <si>
     <t>ns_meta</t>
+  </si>
+  <si>
+    <t>["adfind-pid0001", adfind-pid0009"]</t>
+  </si>
+  <si>
+    <t>["adfind-pid0002", adfind-pid0009"]</t>
+  </si>
+  <si>
+    <t>["adfind-pid0007", adfind-pid0009"]</t>
+  </si>
+  <si>
+    <t>["adfind-pid0008", adfind-pid0009"]</t>
+  </si>
+  <si>
+    <t>ET POLICY OpenSSL Demo CA - Internet Widgits Pty (O)</t>
+  </si>
+  <si>
+    <t>ET POLICY SMB Executable File Transfer</t>
+  </si>
+  <si>
+    <t>ET RPC DCERPC SVCCTL - Remote Service Control Manager Access</t>
+  </si>
+  <si>
+    <t>ET POLICY SMB2 NT Create AndX Request For an Executable File</t>
+  </si>
+  <si>
+    <t>ET POLICY SSL/TLS Certificate Observed (AnyDesk Remote Desktop Software)</t>
+  </si>
+  <si>
+    <t>(Snort VRT) MALWARE-OTHER CobaltStrike powershell web delivery attempt</t>
+  </si>
+  <si>
+    <t>etpro</t>
+  </si>
+  <si>
+    <t>{"sigma_uuid": "4358e5a5-7542-4dcb-b9f3-87667371839b" :  "ISO or Image Mount Indicator in Recent Files"}</t>
+  </si>
+  <si>
+    <t>dfir20220808-eid0106</t>
+  </si>
+  <si>
+    <t>dfir20220808-eid0107</t>
+  </si>
+  <si>
+    <t>dfir20220808-eid0108</t>
+  </si>
+  <si>
+    <t>dfir20220808-eid0109</t>
+  </si>
+  <si>
+    <t>dfir20220808-eid0110</t>
   </si>
 </sst>
 </file>
@@ -813,8 +843,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C77889FB-1522-0A4D-8EB6-D259755FECDF}" name="Table1" displayName="Table1" ref="A1:G107" totalsRowShown="0" dataDxfId="7">
-  <autoFilter ref="A1:G107" xr:uid="{C77889FB-1522-0A4D-8EB6-D259755FECDF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C77889FB-1522-0A4D-8EB6-D259755FECDF}" name="Table1" displayName="Table1" ref="A1:G111" totalsRowShown="0" dataDxfId="7">
+  <autoFilter ref="A1:G111" xr:uid="{C77889FB-1522-0A4D-8EB6-D259755FECDF}"/>
   <tableColumns count="7">
     <tableColumn id="7" xr3:uid="{5516EDED-B058-144E-976C-0B23FABA65AE}" name="eid" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{0B947D48-DA4A-7C49-9C7F-01EFE6AFBBF9}" name="map_pid" dataDxfId="5"/>
@@ -1145,17 +1175,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADA5849-2682-F643-8842-EFF560F6FB5C}">
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.1640625" customWidth="1"/>
     <col min="2" max="2" width="21.5" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="143.33203125" customWidth="1"/>
     <col min="6" max="6" width="82.6640625" customWidth="1"/>
@@ -1173,28 +1203,30 @@
         <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F1" t="s">
         <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>35</v>
@@ -1208,12 +1240,14 @@
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>223</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>40</v>
@@ -1227,12 +1261,14 @@
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>224</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>36</v>
@@ -1246,12 +1282,14 @@
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>225</v>
+      </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>37</v>
@@ -1265,12 +1303,14 @@
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>224</v>
+      </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>38</v>
@@ -1284,12 +1324,14 @@
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>225</v>
+      </c>
       <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>39</v>
@@ -1303,12 +1345,14 @@
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>223</v>
+      </c>
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>34</v>
@@ -1327,7 +1371,7 @@
         <v>11</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>4</v>
@@ -1346,7 +1390,7 @@
         <v>11</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>5</v>
@@ -1365,7 +1409,7 @@
         <v>11</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>6</v>
@@ -1384,7 +1428,7 @@
         <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>7</v>
@@ -1403,7 +1447,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>22</v>
@@ -1420,7 +1464,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>23</v>
@@ -1437,7 +1481,7 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>26</v>
@@ -1454,7 +1498,7 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>27</v>
@@ -1471,7 +1515,7 @@
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>28</v>
@@ -1488,7 +1532,7 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>29</v>
@@ -1505,7 +1549,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>30</v>
@@ -1522,7 +1566,7 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>31</v>
@@ -1539,7 +1583,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>32</v>
@@ -1556,7 +1600,7 @@
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>33</v>
@@ -1573,7 +1617,7 @@
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>41</v>
@@ -1590,7 +1634,7 @@
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>42</v>
@@ -1607,7 +1651,7 @@
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>43</v>
@@ -1624,7 +1668,7 @@
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>44</v>
@@ -1641,7 +1685,7 @@
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>57</v>
@@ -1658,7 +1702,7 @@
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>60</v>
@@ -1675,7 +1719,7 @@
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>59</v>
@@ -1692,7 +1736,7 @@
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>58</v>
@@ -1709,7 +1753,7 @@
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>61</v>
@@ -1726,7 +1770,7 @@
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>62</v>
@@ -1743,7 +1787,7 @@
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>69</v>
@@ -1760,7 +1804,7 @@
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>70</v>
@@ -1777,7 +1821,7 @@
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>71</v>
@@ -1794,7 +1838,7 @@
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>72</v>
@@ -1811,7 +1855,7 @@
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>73</v>
@@ -1828,7 +1872,7 @@
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>74</v>
@@ -1845,7 +1889,7 @@
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>75</v>
@@ -1862,7 +1906,7 @@
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>76</v>
@@ -1879,7 +1923,7 @@
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>85</v>
@@ -1896,7 +1940,7 @@
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>86</v>
@@ -1913,7 +1957,7 @@
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>87</v>
@@ -1930,7 +1974,7 @@
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>88</v>
@@ -1947,7 +1991,7 @@
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>89</v>
@@ -1964,7 +2008,7 @@
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>90</v>
@@ -1981,7 +2025,7 @@
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>91</v>
@@ -1998,7 +2042,7 @@
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>92</v>
@@ -2015,7 +2059,7 @@
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>101</v>
@@ -2032,7 +2076,7 @@
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>102</v>
@@ -2049,7 +2093,7 @@
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>103</v>
@@ -2066,7 +2110,7 @@
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>107</v>
@@ -2083,7 +2127,7 @@
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>112</v>
@@ -2100,7 +2144,7 @@
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>110</v>
@@ -2117,7 +2161,7 @@
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>111</v>
@@ -2134,7 +2178,7 @@
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>113</v>
@@ -2151,7 +2195,7 @@
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>114</v>
@@ -2168,7 +2212,7 @@
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>115</v>
@@ -2185,7 +2229,7 @@
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>116</v>
@@ -2202,7 +2246,7 @@
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>117</v>
@@ -2219,7 +2263,7 @@
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>118</v>
@@ -2236,7 +2280,7 @@
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>119</v>
@@ -2253,7 +2297,7 @@
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>120</v>
@@ -2270,7 +2314,7 @@
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>122</v>
@@ -2287,7 +2331,7 @@
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>121</v>
@@ -2304,7 +2348,7 @@
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>135</v>
@@ -2321,10 +2365,10 @@
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>137</v>
@@ -2340,7 +2384,7 @@
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>140</v>
@@ -2359,7 +2403,7 @@
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>141</v>
@@ -2378,7 +2422,7 @@
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>142</v>
@@ -2397,7 +2441,7 @@
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>143</v>
@@ -2416,7 +2460,7 @@
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>144</v>
@@ -2435,7 +2479,7 @@
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>150</v>
@@ -2454,7 +2498,7 @@
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>151</v>
@@ -2473,7 +2517,7 @@
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>152</v>
@@ -2492,7 +2536,7 @@
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>153</v>
@@ -2511,7 +2555,7 @@
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>154</v>
@@ -2530,7 +2574,7 @@
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>155</v>
@@ -2549,7 +2593,7 @@
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>156</v>
@@ -2568,7 +2612,7 @@
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>157</v>
@@ -2587,7 +2631,7 @@
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>158</v>
@@ -2606,7 +2650,7 @@
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>159</v>
@@ -2625,7 +2669,7 @@
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>160</v>
@@ -2644,7 +2688,7 @@
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>161</v>
@@ -2663,10 +2707,10 @@
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>221</v>
+        <v>174</v>
       </c>
       <c r="F85" s="1"/>
       <c r="G85" s="1" t="s">
@@ -2680,10 +2724,10 @@
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>222</v>
+        <v>175</v>
       </c>
       <c r="F86" s="1"/>
       <c r="G86" s="1" t="s">
@@ -2697,10 +2741,10 @@
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="1" t="s">
@@ -2714,10 +2758,10 @@
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F88" s="1"/>
       <c r="G88" s="1" t="s">
@@ -2731,10 +2775,10 @@
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="F89" s="1"/>
       <c r="G89" s="1" t="s">
@@ -2748,10 +2792,10 @@
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>177</v>
+        <v>233</v>
       </c>
       <c r="F90" s="1"/>
       <c r="G90" s="1" t="s">
@@ -2760,12 +2804,12 @@
     </row>
     <row r="91" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>185</v>
@@ -2777,15 +2821,15 @@
     </row>
     <row r="92" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F92" s="1"/>
       <c r="G92" s="1" t="s">
@@ -2794,15 +2838,15 @@
     </row>
     <row r="93" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F93" s="1"/>
       <c r="G93" s="1" t="s">
@@ -2811,15 +2855,15 @@
     </row>
     <row r="94" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F94" s="1"/>
       <c r="G94" s="1" t="s">
@@ -2828,15 +2872,15 @@
     </row>
     <row r="95" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F95" s="1"/>
       <c r="G95" s="1" t="s">
@@ -2845,15 +2889,15 @@
     </row>
     <row r="96" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="1" t="s">
@@ -2862,15 +2906,15 @@
     </row>
     <row r="97" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F97" s="1"/>
       <c r="G97" s="1" t="s">
@@ -2879,15 +2923,15 @@
     </row>
     <row r="98" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F98" s="1"/>
       <c r="G98" s="1" t="s">
@@ -2896,15 +2940,15 @@
     </row>
     <row r="99" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F99" s="1"/>
       <c r="G99" s="1" t="s">
@@ -2913,15 +2957,15 @@
     </row>
     <row r="100" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F100" s="1"/>
       <c r="G100" s="1" t="s">
@@ -2930,15 +2974,15 @@
     </row>
     <row r="101" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="1" t="s">
@@ -2947,15 +2991,15 @@
     </row>
     <row r="102" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="1" t="s">
@@ -2964,15 +3008,15 @@
     </row>
     <row r="103" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F103" s="1"/>
       <c r="G103" s="1" t="s">
@@ -2981,15 +3025,15 @@
     </row>
     <row r="104" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F104" s="1"/>
       <c r="G104" s="1" t="s">
@@ -2998,50 +3042,108 @@
     </row>
     <row r="105" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>198</v>
+        <v>226</v>
       </c>
       <c r="F105" s="1"/>
-      <c r="G105" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="G105" s="1"/>
     </row>
     <row r="106" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>199</v>
+        <v>227</v>
       </c>
       <c r="F106" s="1"/>
-      <c r="G106" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" ht="119" x14ac:dyDescent="0.2">
-      <c r="A107" s="1"/>
+      <c r="G106" s="1"/>
+    </row>
+    <row r="107" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1" t="s">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
+    </row>
+    <row r="108" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F108" s="1"/>
+      <c r="G108" s="1"/>
+    </row>
+    <row r="109" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A109" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F109" s="1"/>
+      <c r="G109" s="1"/>
+    </row>
+    <row r="110" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F110" s="1"/>
+      <c r="G110" s="1"/>
+    </row>
+    <row r="111" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F111" s="1"/>
+      <c r="G111" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>